<commit_message>
Update epplus related code in epplus.cs.
removed redundant sample data and generated files and code
</commit_message>
<xml_diff>
--- a/packageTestPlan.xlsx
+++ b/packageTestPlan.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\NBURNESS\source\repos\BenchmarkingExcelPackages\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E83263B-5105-4B38-8367-0B98FE93E2FB}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF9B0764-89F1-4BD8-BC9F-8856103EBEDD}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="44880" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{94930DDF-C3E7-4854-A3F2-65E07A382ABF}"/>
+    <workbookView xWindow="48480" yWindow="2565" windowWidth="21600" windowHeight="11145" xr2:uid="{94930DDF-C3E7-4854-A3F2-65E07A382ABF}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -54,9 +54,6 @@
     <t>Can create multiple sheets in newly created file.</t>
   </si>
   <si>
-    <t>Can select a cell by column and row</t>
-  </si>
-  <si>
     <t>Can select all cells in a row</t>
   </si>
   <si>
@@ -99,20 +96,23 @@
     <t>Can find the last row of data and ignore the first row</t>
   </si>
   <si>
-    <t>Notes:- Sample data document used to carry out this test plan contains 2 worksheets, main worksheet contains 100K rows with some records in the first 4 rows.</t>
-  </si>
-  <si>
     <t>TestNo</t>
   </si>
   <si>
     <t>ü</t>
+  </si>
+  <si>
+    <t>Notes:- Sample data document used to carry out this test plan contains 2 worksheets, main worksheet contains 100K rows with data in multiple columns</t>
+  </si>
+  <si>
+    <t>Can select a single cell by column and row</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -140,8 +140,15 @@
       <name val="Wingdings"/>
       <charset val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -158,8 +165,13 @@
         <fgColor rgb="FFFFEB9C"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="20">
+  <borders count="13">
     <border>
       <left/>
       <right/>
@@ -229,23 +241,10 @@
       <left style="medium">
         <color indexed="64"/>
       </left>
-      <right/>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
       <right style="medium">
         <color indexed="64"/>
       </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
+      <top/>
       <bottom style="medium">
         <color indexed="64"/>
       </bottom>
@@ -258,29 +257,26 @@
       <right style="medium">
         <color indexed="64"/>
       </right>
-      <top/>
-      <bottom style="medium">
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right style="medium">
-        <color indexed="64"/>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
       </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="medium">
-        <color indexed="64"/>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -288,24 +284,6 @@
       <left style="medium">
         <color indexed="64"/>
       </left>
-      <right/>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
       <right style="medium">
         <color indexed="64"/>
       </right>
@@ -319,17 +297,40 @@
       <left style="medium">
         <color indexed="64"/>
       </left>
-      <right/>
-      <top/>
-      <bottom/>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
-      <left style="medium">
-        <color indexed="64"/>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
       </left>
       <right/>
-      <top/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
       <bottom style="medium">
         <color indexed="64"/>
       </bottom>
@@ -337,66 +338,25 @@
     </border>
     <border>
       <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="medium">
         <color indexed="64"/>
       </top>
       <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
@@ -404,56 +364,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="10" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="11" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="12" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="13" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="8" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="14" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="15" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="9" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -467,9 +378,38 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="2" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="9" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="11" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="10" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="12" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="4">
     <cellStyle name="Good" xfId="1" builtinId="26"/>
+    <cellStyle name="Input" xfId="3" builtinId="20"/>
     <cellStyle name="Neutral" xfId="2" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
@@ -786,7 +726,7 @@
   <dimension ref="A1:T28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E24" sqref="E24"/>
+      <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -798,28 +738,28 @@
   <sheetData>
     <row r="1" spans="1:20" ht="14.65" thickBot="1" x14ac:dyDescent="0.5"/>
     <row r="2" spans="1:20" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A2" s="14" t="s">
-        <v>22</v>
-      </c>
-      <c r="B2" s="8" t="s">
+      <c r="A2" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="B2" s="19" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="6" t="s">
+      <c r="C2" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="D2" s="16"/>
+      <c r="E2" s="15" t="s">
         <v>17</v>
       </c>
-      <c r="D2" s="7"/>
-      <c r="E2" s="6" t="s">
+      <c r="F2" s="17"/>
+      <c r="G2" s="18" t="s">
         <v>18</v>
       </c>
-      <c r="F2" s="7"/>
-      <c r="G2" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="H2" s="7"/>
+      <c r="H2" s="17"/>
     </row>
     <row r="3" spans="1:20" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A3" s="15"/>
-      <c r="B3" s="9"/>
+      <c r="A3" s="13"/>
+      <c r="B3" s="20"/>
       <c r="C3" s="4" t="s">
         <v>1</v>
       </c>
@@ -840,10 +780,10 @@
       </c>
     </row>
     <row r="4" spans="1:20" x14ac:dyDescent="0.45">
-      <c r="A4" s="27">
+      <c r="A4" s="8">
         <v>1.1000000000000001</v>
       </c>
-      <c r="B4" s="10" t="s">
+      <c r="B4" s="1" t="s">
         <v>3</v>
       </c>
       <c r="C4" s="1" t="b">
@@ -853,17 +793,17 @@
       <c r="E4" s="1" t="b">
         <v>1</v>
       </c>
-      <c r="F4" s="25" t="b">
+      <c r="F4" s="6" t="b">
         <v>1</v>
       </c>
       <c r="G4" s="1"/>
       <c r="H4" s="1"/>
     </row>
     <row r="5" spans="1:20" x14ac:dyDescent="0.45">
-      <c r="A5" s="28">
+      <c r="A5" s="9">
         <v>1.2</v>
       </c>
-      <c r="B5" s="11" t="s">
+      <c r="B5" s="2" t="s">
         <v>4</v>
       </c>
       <c r="C5" s="1" t="b">
@@ -873,17 +813,17 @@
       <c r="E5" s="1" t="b">
         <v>1</v>
       </c>
-      <c r="F5" s="25" t="b">
+      <c r="F5" s="6" t="b">
         <v>1</v>
       </c>
       <c r="G5" s="1"/>
       <c r="H5" s="1"/>
     </row>
     <row r="6" spans="1:20" x14ac:dyDescent="0.45">
-      <c r="A6" s="28">
+      <c r="A6" s="9">
         <v>1.3</v>
       </c>
-      <c r="B6" s="11" t="s">
+      <c r="B6" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C6" s="1" t="b">
@@ -893,18 +833,18 @@
       <c r="E6" s="1" t="b">
         <v>1</v>
       </c>
-      <c r="F6" s="25" t="b">
+      <c r="F6" s="6" t="b">
         <v>1</v>
       </c>
       <c r="G6" s="1"/>
       <c r="H6" s="1"/>
     </row>
     <row r="7" spans="1:20" x14ac:dyDescent="0.45">
-      <c r="A7" s="28">
+      <c r="A7" s="9">
         <v>1.4</v>
       </c>
-      <c r="B7" s="11" t="s">
-        <v>6</v>
+      <c r="B7" s="2" t="s">
+        <v>23</v>
       </c>
       <c r="C7" s="1" t="b">
         <v>1</v>
@@ -913,18 +853,18 @@
       <c r="E7" s="1" t="b">
         <v>1</v>
       </c>
-      <c r="F7" s="25" t="b">
+      <c r="F7" s="6" t="b">
         <v>1</v>
       </c>
       <c r="G7" s="1"/>
       <c r="H7" s="1"/>
     </row>
     <row r="8" spans="1:20" x14ac:dyDescent="0.45">
-      <c r="A8" s="28">
+      <c r="A8" s="9">
         <v>1.5</v>
       </c>
-      <c r="B8" s="11" t="s">
-        <v>7</v>
+      <c r="B8" s="2" t="s">
+        <v>6</v>
       </c>
       <c r="C8" s="1" t="b">
         <v>1</v>
@@ -933,18 +873,18 @@
       <c r="E8" s="1" t="b">
         <v>1</v>
       </c>
-      <c r="F8" s="25" t="b">
+      <c r="F8" s="6" t="b">
         <v>1</v>
       </c>
       <c r="G8" s="1"/>
       <c r="H8" s="1"/>
     </row>
     <row r="9" spans="1:20" x14ac:dyDescent="0.45">
-      <c r="A9" s="28">
+      <c r="A9" s="9">
         <v>1.6</v>
       </c>
-      <c r="B9" s="11" t="s">
-        <v>20</v>
+      <c r="B9" s="2" t="s">
+        <v>19</v>
       </c>
       <c r="C9" s="1" t="b">
         <v>1</v>
@@ -953,18 +893,18 @@
       <c r="E9" s="1" t="b">
         <v>1</v>
       </c>
-      <c r="F9" s="25" t="b">
+      <c r="F9" s="6" t="b">
         <v>1</v>
       </c>
       <c r="G9" s="1"/>
       <c r="H9" s="1"/>
     </row>
     <row r="10" spans="1:20" x14ac:dyDescent="0.45">
-      <c r="A10" s="28">
+      <c r="A10" s="9">
         <v>1.7</v>
       </c>
-      <c r="B10" s="11" t="s">
-        <v>8</v>
+      <c r="B10" s="2" t="s">
+        <v>7</v>
       </c>
       <c r="C10" s="1" t="b">
         <v>1</v>
@@ -978,11 +918,11 @@
       <c r="H10" s="1"/>
     </row>
     <row r="11" spans="1:20" x14ac:dyDescent="0.45">
-      <c r="A11" s="28">
+      <c r="A11" s="9">
         <v>1.8</v>
       </c>
-      <c r="B11" s="12" t="s">
-        <v>9</v>
+      <c r="B11" s="11" t="s">
+        <v>8</v>
       </c>
       <c r="C11" s="1" t="b">
         <v>1</v>
@@ -991,18 +931,18 @@
       <c r="E11" s="1" t="b">
         <v>1</v>
       </c>
-      <c r="F11" s="25" t="b">
+      <c r="F11" s="6" t="b">
         <v>1</v>
       </c>
       <c r="G11" s="1"/>
       <c r="H11" s="1"/>
     </row>
     <row r="12" spans="1:20" x14ac:dyDescent="0.45">
-      <c r="A12" s="28">
+      <c r="A12" s="9">
         <v>1.9</v>
       </c>
-      <c r="B12" s="11" t="s">
-        <v>10</v>
+      <c r="B12" s="2" t="s">
+        <v>9</v>
       </c>
       <c r="C12" s="1" t="b">
         <v>1</v>
@@ -1011,18 +951,18 @@
       <c r="E12" s="1" t="b">
         <v>1</v>
       </c>
-      <c r="F12" s="26" t="s">
-        <v>23</v>
+      <c r="F12" s="7" t="s">
+        <v>21</v>
       </c>
       <c r="G12" s="1"/>
       <c r="H12" s="1"/>
     </row>
     <row r="13" spans="1:20" x14ac:dyDescent="0.45">
-      <c r="A13" s="28">
+      <c r="A13" s="9">
         <v>2</v>
       </c>
-      <c r="B13" s="11" t="s">
-        <v>11</v>
+      <c r="B13" s="2" t="s">
+        <v>10</v>
       </c>
       <c r="C13" s="1" t="b">
         <v>1</v>
@@ -1031,18 +971,18 @@
       <c r="E13" s="1" t="b">
         <v>1</v>
       </c>
-      <c r="F13" s="25" t="b">
+      <c r="F13" s="6" t="b">
         <v>1</v>
       </c>
       <c r="G13" s="1"/>
       <c r="H13" s="1"/>
     </row>
-    <row r="14" spans="1:20" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A14" s="28">
+    <row r="14" spans="1:20" x14ac:dyDescent="0.45">
+      <c r="A14" s="9">
         <v>2.1</v>
       </c>
-      <c r="B14" s="11" t="s">
-        <v>12</v>
+      <c r="B14" s="2" t="s">
+        <v>11</v>
       </c>
       <c r="C14" s="1" t="b">
         <v>1</v>
@@ -1051,18 +991,18 @@
       <c r="E14" s="1" t="b">
         <v>1</v>
       </c>
-      <c r="F14" s="25" t="b">
+      <c r="F14" s="6" t="b">
         <v>1</v>
       </c>
       <c r="G14" s="1"/>
       <c r="H14" s="1"/>
     </row>
     <row r="15" spans="1:20" x14ac:dyDescent="0.45">
-      <c r="A15" s="28">
+      <c r="A15" s="9">
         <v>2.2000000000000002</v>
       </c>
-      <c r="B15" s="11" t="s">
-        <v>13</v>
+      <c r="B15" s="2" t="s">
+        <v>12</v>
       </c>
       <c r="C15" s="1" t="b">
         <v>1</v>
@@ -1071,31 +1011,31 @@
       <c r="E15" s="1" t="b">
         <v>1</v>
       </c>
-      <c r="F15" s="25" t="b">
+      <c r="F15" s="6" t="b">
         <v>1</v>
       </c>
       <c r="G15" s="1"/>
       <c r="H15" s="1"/>
-      <c r="J15" s="16" t="s">
-        <v>21</v>
-      </c>
-      <c r="K15" s="17"/>
-      <c r="L15" s="17"/>
-      <c r="M15" s="17"/>
-      <c r="N15" s="17"/>
-      <c r="O15" s="17"/>
-      <c r="P15" s="17"/>
-      <c r="Q15" s="17"/>
-      <c r="R15" s="17"/>
-      <c r="S15" s="17"/>
-      <c r="T15" s="18"/>
+      <c r="J15" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="K15" s="14"/>
+      <c r="L15" s="14"/>
+      <c r="M15" s="14"/>
+      <c r="N15" s="14"/>
+      <c r="O15" s="14"/>
+      <c r="P15" s="14"/>
+      <c r="Q15" s="14"/>
+      <c r="R15" s="14"/>
+      <c r="S15" s="14"/>
+      <c r="T15" s="14"/>
     </row>
     <row r="16" spans="1:20" x14ac:dyDescent="0.45">
-      <c r="A16" s="28">
+      <c r="A16" s="9">
         <v>2.2999999999999998</v>
       </c>
-      <c r="B16" s="11" t="s">
-        <v>14</v>
+      <c r="B16" s="2" t="s">
+        <v>13</v>
       </c>
       <c r="C16" s="1" t="b">
         <v>1</v>
@@ -1104,29 +1044,29 @@
       <c r="E16" s="1" t="b">
         <v>1</v>
       </c>
-      <c r="F16" s="25" t="b">
+      <c r="F16" s="6" t="b">
         <v>1</v>
       </c>
       <c r="G16" s="1"/>
       <c r="H16" s="1"/>
-      <c r="J16" s="19"/>
-      <c r="K16" s="20"/>
-      <c r="L16" s="20"/>
-      <c r="M16" s="20"/>
-      <c r="N16" s="20"/>
-      <c r="O16" s="20"/>
-      <c r="P16" s="20"/>
-      <c r="Q16" s="20"/>
-      <c r="R16" s="20"/>
-      <c r="S16" s="20"/>
-      <c r="T16" s="21"/>
+      <c r="J16" s="14"/>
+      <c r="K16" s="14"/>
+      <c r="L16" s="14"/>
+      <c r="M16" s="14"/>
+      <c r="N16" s="14"/>
+      <c r="O16" s="14"/>
+      <c r="P16" s="14"/>
+      <c r="Q16" s="14"/>
+      <c r="R16" s="14"/>
+      <c r="S16" s="14"/>
+      <c r="T16" s="14"/>
     </row>
     <row r="17" spans="1:20" x14ac:dyDescent="0.45">
-      <c r="A17" s="28">
+      <c r="A17" s="9">
         <v>2.4</v>
       </c>
-      <c r="B17" s="11" t="s">
-        <v>15</v>
+      <c r="B17" s="2" t="s">
+        <v>14</v>
       </c>
       <c r="C17" s="1" t="b">
         <v>1</v>
@@ -1135,29 +1075,29 @@
       <c r="E17" s="1" t="b">
         <v>1</v>
       </c>
-      <c r="F17" s="25" t="b">
+      <c r="F17" s="6" t="b">
         <v>1</v>
       </c>
       <c r="G17" s="1"/>
       <c r="H17" s="1"/>
-      <c r="J17" s="19"/>
-      <c r="K17" s="20"/>
-      <c r="L17" s="20"/>
-      <c r="M17" s="20"/>
-      <c r="N17" s="20"/>
-      <c r="O17" s="20"/>
-      <c r="P17" s="20"/>
-      <c r="Q17" s="20"/>
-      <c r="R17" s="20"/>
-      <c r="S17" s="20"/>
-      <c r="T17" s="21"/>
+      <c r="J17" s="14"/>
+      <c r="K17" s="14"/>
+      <c r="L17" s="14"/>
+      <c r="M17" s="14"/>
+      <c r="N17" s="14"/>
+      <c r="O17" s="14"/>
+      <c r="P17" s="14"/>
+      <c r="Q17" s="14"/>
+      <c r="R17" s="14"/>
+      <c r="S17" s="14"/>
+      <c r="T17" s="14"/>
     </row>
     <row r="18" spans="1:20" x14ac:dyDescent="0.45">
-      <c r="A18" s="28">
+      <c r="A18" s="9">
         <v>2.5</v>
       </c>
-      <c r="B18" s="11" t="s">
-        <v>16</v>
+      <c r="B18" s="2" t="s">
+        <v>15</v>
       </c>
       <c r="C18" s="1" t="b">
         <v>1</v>
@@ -1166,232 +1106,232 @@
       <c r="E18" s="1" t="b">
         <v>1</v>
       </c>
-      <c r="F18" s="25" t="b">
+      <c r="F18" s="6" t="b">
         <v>1</v>
       </c>
       <c r="G18" s="1"/>
       <c r="H18" s="1"/>
-      <c r="J18" s="19"/>
-      <c r="K18" s="20"/>
-      <c r="L18" s="20"/>
-      <c r="M18" s="20"/>
-      <c r="N18" s="20"/>
-      <c r="O18" s="20"/>
-      <c r="P18" s="20"/>
-      <c r="Q18" s="20"/>
-      <c r="R18" s="20"/>
-      <c r="S18" s="20"/>
-      <c r="T18" s="21"/>
+      <c r="J18" s="14"/>
+      <c r="K18" s="14"/>
+      <c r="L18" s="14"/>
+      <c r="M18" s="14"/>
+      <c r="N18" s="14"/>
+      <c r="O18" s="14"/>
+      <c r="P18" s="14"/>
+      <c r="Q18" s="14"/>
+      <c r="R18" s="14"/>
+      <c r="S18" s="14"/>
+      <c r="T18" s="14"/>
     </row>
     <row r="19" spans="1:20" x14ac:dyDescent="0.45">
-      <c r="A19" s="28"/>
-      <c r="B19" s="11"/>
+      <c r="A19" s="9"/>
+      <c r="B19" s="2"/>
       <c r="C19" s="2"/>
       <c r="D19" s="2"/>
       <c r="E19" s="1"/>
       <c r="F19" s="1"/>
       <c r="G19" s="1"/>
       <c r="H19" s="1"/>
-      <c r="J19" s="19"/>
-      <c r="K19" s="20"/>
-      <c r="L19" s="20"/>
-      <c r="M19" s="20"/>
-      <c r="N19" s="20"/>
-      <c r="O19" s="20"/>
-      <c r="P19" s="20"/>
-      <c r="Q19" s="20"/>
-      <c r="R19" s="20"/>
-      <c r="S19" s="20"/>
-      <c r="T19" s="21"/>
+      <c r="J19" s="14"/>
+      <c r="K19" s="14"/>
+      <c r="L19" s="14"/>
+      <c r="M19" s="14"/>
+      <c r="N19" s="14"/>
+      <c r="O19" s="14"/>
+      <c r="P19" s="14"/>
+      <c r="Q19" s="14"/>
+      <c r="R19" s="14"/>
+      <c r="S19" s="14"/>
+      <c r="T19" s="14"/>
     </row>
     <row r="20" spans="1:20" x14ac:dyDescent="0.45">
-      <c r="A20" s="28"/>
-      <c r="B20" s="11"/>
+      <c r="A20" s="9"/>
+      <c r="B20" s="2"/>
       <c r="C20" s="2"/>
       <c r="D20" s="2"/>
       <c r="E20" s="1"/>
       <c r="F20" s="1"/>
       <c r="G20" s="1"/>
       <c r="H20" s="1"/>
-      <c r="J20" s="19"/>
-      <c r="K20" s="20"/>
-      <c r="L20" s="20"/>
-      <c r="M20" s="20"/>
-      <c r="N20" s="20"/>
-      <c r="O20" s="20"/>
-      <c r="P20" s="20"/>
-      <c r="Q20" s="20"/>
-      <c r="R20" s="20"/>
-      <c r="S20" s="20"/>
-      <c r="T20" s="21"/>
+      <c r="J20" s="14"/>
+      <c r="K20" s="14"/>
+      <c r="L20" s="14"/>
+      <c r="M20" s="14"/>
+      <c r="N20" s="14"/>
+      <c r="O20" s="14"/>
+      <c r="P20" s="14"/>
+      <c r="Q20" s="14"/>
+      <c r="R20" s="14"/>
+      <c r="S20" s="14"/>
+      <c r="T20" s="14"/>
     </row>
     <row r="21" spans="1:20" x14ac:dyDescent="0.45">
-      <c r="A21" s="28"/>
-      <c r="B21" s="11"/>
+      <c r="A21" s="9"/>
+      <c r="B21" s="2"/>
       <c r="C21" s="2"/>
       <c r="D21" s="2"/>
       <c r="E21" s="1"/>
       <c r="F21" s="1"/>
       <c r="G21" s="1"/>
       <c r="H21" s="1"/>
-      <c r="J21" s="19"/>
-      <c r="K21" s="20"/>
-      <c r="L21" s="20"/>
-      <c r="M21" s="20"/>
-      <c r="N21" s="20"/>
-      <c r="O21" s="20"/>
-      <c r="P21" s="20"/>
-      <c r="Q21" s="20"/>
-      <c r="R21" s="20"/>
-      <c r="S21" s="20"/>
-      <c r="T21" s="21"/>
+      <c r="J21" s="14"/>
+      <c r="K21" s="14"/>
+      <c r="L21" s="14"/>
+      <c r="M21" s="14"/>
+      <c r="N21" s="14"/>
+      <c r="O21" s="14"/>
+      <c r="P21" s="14"/>
+      <c r="Q21" s="14"/>
+      <c r="R21" s="14"/>
+      <c r="S21" s="14"/>
+      <c r="T21" s="14"/>
     </row>
     <row r="22" spans="1:20" x14ac:dyDescent="0.45">
-      <c r="A22" s="28"/>
-      <c r="B22" s="11"/>
+      <c r="A22" s="9"/>
+      <c r="B22" s="2"/>
       <c r="C22" s="2"/>
       <c r="D22" s="2"/>
       <c r="E22" s="1"/>
       <c r="F22" s="1"/>
       <c r="G22" s="1"/>
       <c r="H22" s="1"/>
-      <c r="J22" s="19"/>
-      <c r="K22" s="20"/>
-      <c r="L22" s="20"/>
-      <c r="M22" s="20"/>
-      <c r="N22" s="20"/>
-      <c r="O22" s="20"/>
-      <c r="P22" s="20"/>
-      <c r="Q22" s="20"/>
-      <c r="R22" s="20"/>
-      <c r="S22" s="20"/>
-      <c r="T22" s="21"/>
+      <c r="J22" s="14"/>
+      <c r="K22" s="14"/>
+      <c r="L22" s="14"/>
+      <c r="M22" s="14"/>
+      <c r="N22" s="14"/>
+      <c r="O22" s="14"/>
+      <c r="P22" s="14"/>
+      <c r="Q22" s="14"/>
+      <c r="R22" s="14"/>
+      <c r="S22" s="14"/>
+      <c r="T22" s="14"/>
     </row>
     <row r="23" spans="1:20" x14ac:dyDescent="0.45">
-      <c r="A23" s="28"/>
-      <c r="B23" s="11"/>
+      <c r="A23" s="9"/>
+      <c r="B23" s="2"/>
       <c r="C23" s="2"/>
       <c r="D23" s="2"/>
       <c r="E23" s="1"/>
       <c r="F23" s="1"/>
       <c r="G23" s="1"/>
       <c r="H23" s="1"/>
-      <c r="J23" s="19"/>
-      <c r="K23" s="20"/>
-      <c r="L23" s="20"/>
-      <c r="M23" s="20"/>
-      <c r="N23" s="20"/>
-      <c r="O23" s="20"/>
-      <c r="P23" s="20"/>
-      <c r="Q23" s="20"/>
-      <c r="R23" s="20"/>
-      <c r="S23" s="20"/>
-      <c r="T23" s="21"/>
+      <c r="J23" s="14"/>
+      <c r="K23" s="14"/>
+      <c r="L23" s="14"/>
+      <c r="M23" s="14"/>
+      <c r="N23" s="14"/>
+      <c r="O23" s="14"/>
+      <c r="P23" s="14"/>
+      <c r="Q23" s="14"/>
+      <c r="R23" s="14"/>
+      <c r="S23" s="14"/>
+      <c r="T23" s="14"/>
     </row>
     <row r="24" spans="1:20" x14ac:dyDescent="0.45">
-      <c r="A24" s="28"/>
-      <c r="B24" s="11"/>
+      <c r="A24" s="9"/>
+      <c r="B24" s="2"/>
       <c r="C24" s="2"/>
       <c r="D24" s="2"/>
       <c r="E24" s="1"/>
       <c r="F24" s="1"/>
       <c r="G24" s="1"/>
       <c r="H24" s="1"/>
-      <c r="J24" s="19"/>
-      <c r="K24" s="20"/>
-      <c r="L24" s="20"/>
-      <c r="M24" s="20"/>
-      <c r="N24" s="20"/>
-      <c r="O24" s="20"/>
-      <c r="P24" s="20"/>
-      <c r="Q24" s="20"/>
-      <c r="R24" s="20"/>
-      <c r="S24" s="20"/>
-      <c r="T24" s="21"/>
+      <c r="J24" s="14"/>
+      <c r="K24" s="14"/>
+      <c r="L24" s="14"/>
+      <c r="M24" s="14"/>
+      <c r="N24" s="14"/>
+      <c r="O24" s="14"/>
+      <c r="P24" s="14"/>
+      <c r="Q24" s="14"/>
+      <c r="R24" s="14"/>
+      <c r="S24" s="14"/>
+      <c r="T24" s="14"/>
     </row>
     <row r="25" spans="1:20" x14ac:dyDescent="0.45">
-      <c r="A25" s="28"/>
-      <c r="B25" s="11"/>
+      <c r="A25" s="9"/>
+      <c r="B25" s="2"/>
       <c r="C25" s="2"/>
       <c r="D25" s="2"/>
       <c r="E25" s="1"/>
       <c r="F25" s="1"/>
       <c r="G25" s="1"/>
       <c r="H25" s="1"/>
-      <c r="J25" s="19"/>
-      <c r="K25" s="20"/>
-      <c r="L25" s="20"/>
-      <c r="M25" s="20"/>
-      <c r="N25" s="20"/>
-      <c r="O25" s="20"/>
-      <c r="P25" s="20"/>
-      <c r="Q25" s="20"/>
-      <c r="R25" s="20"/>
-      <c r="S25" s="20"/>
-      <c r="T25" s="21"/>
+      <c r="J25" s="14"/>
+      <c r="K25" s="14"/>
+      <c r="L25" s="14"/>
+      <c r="M25" s="14"/>
+      <c r="N25" s="14"/>
+      <c r="O25" s="14"/>
+      <c r="P25" s="14"/>
+      <c r="Q25" s="14"/>
+      <c r="R25" s="14"/>
+      <c r="S25" s="14"/>
+      <c r="T25" s="14"/>
     </row>
     <row r="26" spans="1:20" x14ac:dyDescent="0.45">
-      <c r="A26" s="28"/>
-      <c r="B26" s="11"/>
+      <c r="A26" s="9"/>
+      <c r="B26" s="2"/>
       <c r="C26" s="2"/>
       <c r="D26" s="2"/>
       <c r="E26" s="1"/>
       <c r="F26" s="1"/>
       <c r="G26" s="1"/>
       <c r="H26" s="1"/>
-      <c r="J26" s="19"/>
-      <c r="K26" s="20"/>
-      <c r="L26" s="20"/>
-      <c r="M26" s="20"/>
-      <c r="N26" s="20"/>
-      <c r="O26" s="20"/>
-      <c r="P26" s="20"/>
-      <c r="Q26" s="20"/>
-      <c r="R26" s="20"/>
-      <c r="S26" s="20"/>
-      <c r="T26" s="21"/>
+      <c r="J26" s="14"/>
+      <c r="K26" s="14"/>
+      <c r="L26" s="14"/>
+      <c r="M26" s="14"/>
+      <c r="N26" s="14"/>
+      <c r="O26" s="14"/>
+      <c r="P26" s="14"/>
+      <c r="Q26" s="14"/>
+      <c r="R26" s="14"/>
+      <c r="S26" s="14"/>
+      <c r="T26" s="14"/>
     </row>
     <row r="27" spans="1:20" x14ac:dyDescent="0.45">
-      <c r="A27" s="28"/>
-      <c r="B27" s="11"/>
+      <c r="A27" s="9"/>
+      <c r="B27" s="2"/>
       <c r="C27" s="2"/>
       <c r="D27" s="2"/>
       <c r="E27" s="1"/>
       <c r="F27" s="1"/>
       <c r="G27" s="1"/>
       <c r="H27" s="1"/>
-      <c r="J27" s="19"/>
-      <c r="K27" s="20"/>
-      <c r="L27" s="20"/>
-      <c r="M27" s="20"/>
-      <c r="N27" s="20"/>
-      <c r="O27" s="20"/>
-      <c r="P27" s="20"/>
-      <c r="Q27" s="20"/>
-      <c r="R27" s="20"/>
-      <c r="S27" s="20"/>
-      <c r="T27" s="21"/>
+      <c r="J27" s="14"/>
+      <c r="K27" s="14"/>
+      <c r="L27" s="14"/>
+      <c r="M27" s="14"/>
+      <c r="N27" s="14"/>
+      <c r="O27" s="14"/>
+      <c r="P27" s="14"/>
+      <c r="Q27" s="14"/>
+      <c r="R27" s="14"/>
+      <c r="S27" s="14"/>
+      <c r="T27" s="14"/>
     </row>
     <row r="28" spans="1:20" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A28" s="29"/>
-      <c r="B28" s="13"/>
+      <c r="A28" s="10"/>
+      <c r="B28" s="3"/>
       <c r="C28" s="3"/>
       <c r="D28" s="3"/>
       <c r="E28" s="5"/>
       <c r="F28" s="5"/>
       <c r="G28" s="5"/>
       <c r="H28" s="5"/>
-      <c r="J28" s="22"/>
-      <c r="K28" s="23"/>
-      <c r="L28" s="23"/>
-      <c r="M28" s="23"/>
-      <c r="N28" s="23"/>
-      <c r="O28" s="23"/>
-      <c r="P28" s="23"/>
-      <c r="Q28" s="23"/>
-      <c r="R28" s="23"/>
-      <c r="S28" s="23"/>
-      <c r="T28" s="24"/>
+      <c r="J28" s="14"/>
+      <c r="K28" s="14"/>
+      <c r="L28" s="14"/>
+      <c r="M28" s="14"/>
+      <c r="N28" s="14"/>
+      <c r="O28" s="14"/>
+      <c r="P28" s="14"/>
+      <c r="Q28" s="14"/>
+      <c r="R28" s="14"/>
+      <c r="S28" s="14"/>
+      <c r="T28" s="14"/>
     </row>
   </sheetData>
   <mergeCells count="6">

</xml_diff>